<commit_message>
up cham cong dac biet
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/Chấm công.xlsx
+++ b/ASP.NET CORE/HRMNS/Chấm công.xlsx
@@ -211,6 +211,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -220,10 +224,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,7 +531,7 @@
   <dimension ref="B3:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,12 +543,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -687,15 +687,15 @@
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
+      <c r="B17" s="4">
         <v>4</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H17" t="s">
@@ -703,15 +703,15 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="7">
+      <c r="B18" s="4">
         <v>5</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H18" t="s">

</xml_diff>